<commit_message>
Fix a error at 1N4148 diode string
</commit_message>
<xml_diff>
--- a/Assets/Batch Register Parts/Batch Build.xlsx
+++ b/Assets/Batch Register Parts/Batch Build.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PartsHunter\Assets\Batch Register Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96984BE8-D480-4A8C-860F-DE0BAE5114A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20E77FC-1555-4D61-9511-0D2FDFAAFA75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{EA03BA3F-EF08-4D3E-B130-CAB43F857BBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="3" xr2:uid="{EA03BA3F-EF08-4D3E-B130-CAB43F857BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="RESISTOR PTH" sheetId="2" r:id="rId1"/>
@@ -537,9 +537,6 @@
     <t>(Rectifier) 1A</t>
   </si>
   <si>
-    <t>(Signal) 0,3A</t>
-  </si>
-  <si>
     <t>1N5399</t>
   </si>
   <si>
@@ -655,6 +652,9 @@
   </si>
   <si>
     <t>TRIMPOTS</t>
+  </si>
+  <si>
+    <t>(Signal) 0.3A</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7122DCE7-FDF0-4C23-88EA-E5B3B027966C}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
@@ -1032,7 +1032,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>35</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>36</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>38</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>40</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>41</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>44</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>45</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>46</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>48</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>51</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>52</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>53</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>54</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>55</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>56</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>57</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>58</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>59</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>60</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>61</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>62</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>63</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>64</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>65</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>66</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>67</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>68</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>69</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>70</v>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>71</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>72</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>73</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>74</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>75</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>76</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>77</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>78</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>79</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>80</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>81</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>82</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>83</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>84</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>85</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>86</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>87</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>88</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>89</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>90</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>91</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>92</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>93</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>94</v>
@@ -2292,7 +2292,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>95</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>96</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>97</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>98</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>99</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>100</v>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>101</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>102</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>103</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>104</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>105</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>106</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>107</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>108</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>109</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>110</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>111</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>112</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>113</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>114</v>
@@ -2712,7 +2712,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>115</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>116</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>117</v>
@@ -2775,7 +2775,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>118</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>119</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>120</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>121</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>122</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>123</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>124</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>125</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>126</v>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>127</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>128</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>129</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>130</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>131</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>132</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>133</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>134</v>
@@ -3157,7 +3157,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
@@ -3598,7 +3598,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>28</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>29</v>
@@ -3745,7 +3745,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>30</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>34</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>135</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>136</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>137</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>138</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>139</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>140</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>141</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>142</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>143</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>144</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>145</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>146</v>
@@ -4106,7 +4106,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>148</v>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -4148,7 +4148,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>82</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>149</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>96</v>
@@ -4211,7 +4211,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>100</v>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>150</v>
@@ -4253,7 +4253,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>115</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>119</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>131</v>
@@ -4323,8 +4323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869B2999-9EDC-43C8-A93C-53379E3298B9}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4349,7 +4349,7 @@
         <v>162</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="G1" s="1" t="str">
         <f>_xlfn.CONCAT(A1,",",B1," ", C1, " ",D1,",",E1)</f>
-        <v>DIODES,1N4148 (Signal) 0,3A PTH,155</v>
+        <v>DIODES,1N4148 (Signal) 0.3A PTH,155</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4391,7 +4391,7 @@
         <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -4409,10 +4409,10 @@
         <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
@@ -4430,10 +4430,10 @@
         <v>161</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -4451,10 +4451,10 @@
         <v>161</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
@@ -4472,10 +4472,10 @@
         <v>161</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -4493,10 +4493,10 @@
         <v>161</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -4514,10 +4514,10 @@
         <v>161</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1</v>
@@ -4535,10 +4535,10 @@
         <v>161</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -4556,10 +4556,10 @@
         <v>161</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
@@ -4577,10 +4577,10 @@
         <v>161</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
@@ -4598,10 +4598,10 @@
         <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -4619,10 +4619,10 @@
         <v>161</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -4640,10 +4640,10 @@
         <v>161</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -4661,10 +4661,10 @@
         <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -4682,10 +4682,10 @@
         <v>161</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -4703,10 +4703,10 @@
         <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -4724,10 +4724,10 @@
         <v>161</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -4745,10 +4745,10 @@
         <v>161</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -4766,10 +4766,10 @@
         <v>161</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
@@ -4787,10 +4787,10 @@
         <v>161</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -4805,13 +4805,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -4826,13 +4826,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -4847,13 +4847,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>1</v>
@@ -4868,13 +4868,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1</v>
@@ -4889,13 +4889,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -4910,13 +4910,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>1</v>
@@ -4931,13 +4931,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>1</v>
@@ -4952,13 +4952,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -4973,13 +4973,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>1</v>
@@ -4994,13 +4994,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
New passive components added
</commit_message>
<xml_diff>
--- a/Assets/Batch Register Parts/Batch Build.xlsx
+++ b/Assets/Batch Register Parts/Batch Build.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PartsHunter\Assets\Batch Register Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B4C047-6834-4CE2-BCC0-B0890FAFF4CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F489A76-35E2-4A07-B0E9-D2C31D422278}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="28776" windowHeight="16176" activeTab="2" xr2:uid="{EA03BA3F-EF08-4D3E-B130-CAB43F857BBF}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2913" uniqueCount="560">
   <si>
     <t>1/2W</t>
   </si>
@@ -1691,6 +1691,39 @@
   </si>
   <si>
     <t>6.3V 5% Ceramic</t>
+  </si>
+  <si>
+    <t>220uF 25V</t>
+  </si>
+  <si>
+    <t>330uF 35V</t>
+  </si>
+  <si>
+    <t>330uF 16V</t>
+  </si>
+  <si>
+    <t>470uF 35V</t>
+  </si>
+  <si>
+    <t>470uF 16V</t>
+  </si>
+  <si>
+    <t>680uF 16V</t>
+  </si>
+  <si>
+    <t>1000uF 10V</t>
+  </si>
+  <si>
+    <t>1500uF 6.3V</t>
+  </si>
+  <si>
+    <t>6x5 Electrolytic</t>
+  </si>
+  <si>
+    <t>8x10 Electrolytic</t>
+  </si>
+  <si>
+    <t>10x10 Electrolytic</t>
   </si>
 </sst>
 </file>
@@ -9922,10 +9955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBACCCA-E4A7-4298-9222-BB383B67ECE7}">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G168" sqref="G1:G168"/>
+    <sheetView topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12554,7 +12587,7 @@
       </c>
       <c r="F121" s="7"/>
       <c r="G121" s="7" t="str">
-        <f t="shared" ref="G121:G168" si="3">_xlfn.CONCAT(A121,",",B121," ", C121, " ",D121,",",E121)</f>
+        <f t="shared" ref="G121:G169" si="3">_xlfn.CONCAT(A121,",",B121," ", C121, " ",D121,",",E121)</f>
         <v>CAPACITORS,36pF 50V 5% Ceramic 0805 SMD,451</v>
       </c>
     </row>
@@ -13562,40 +13595,278 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D169" s="7"/>
+      <c r="A169" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E169" s="7">
+        <v>499</v>
+      </c>
+      <c r="F169" s="7"/>
+      <c r="G169" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>CAPACITORS,10uF 50V 6x5 Electrolytic SMD,499</v>
+      </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D170" s="7"/>
+      <c r="A170" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E170" s="7">
+        <v>500</v>
+      </c>
+      <c r="F170" s="7"/>
+      <c r="G170" s="7" t="str">
+        <f t="shared" ref="G170" si="4">_xlfn.CONCAT(A170,",",B170," ", C170, " ",D170,",",E170)</f>
+        <v>CAPACITORS,100uF 50V 8x10 Electrolytic SMD,500</v>
+      </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D171" s="7"/>
+      <c r="A171" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E171" s="7">
+        <v>501</v>
+      </c>
+      <c r="F171" s="7"/>
+      <c r="G171" s="7" t="str">
+        <f t="shared" ref="G171:G184" si="5">_xlfn.CONCAT(A171,",",B171," ", C171, " ",D171,",",E171)</f>
+        <v>CAPACITORS,220uF 25V 8x10 Electrolytic SMD,501</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D172" s="7"/>
+      <c r="A172" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="D172" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E172" s="7">
+        <v>502</v>
+      </c>
+      <c r="F172" s="7"/>
+      <c r="G172" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,330uF 35V 10x10 Electrolytic SMD,502</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D173" s="7"/>
+      <c r="A173" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E173" s="7">
+        <v>503</v>
+      </c>
+      <c r="F173" s="7"/>
+      <c r="G173" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,330uF 16V 8x10 Electrolytic SMD,503</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D174" s="7"/>
+      <c r="A174" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E174" s="7">
+        <v>504</v>
+      </c>
+      <c r="F174" s="7"/>
+      <c r="G174" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,470uF 35V 10x10 Electrolytic SMD,504</v>
+      </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D175" s="7"/>
+      <c r="A175" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E175" s="7">
+        <v>505</v>
+      </c>
+      <c r="F175" s="7"/>
+      <c r="G175" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,470uF 16V 8x10 Electrolytic SMD,505</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D176" s="7"/>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D177" s="7"/>
-    </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D178" s="7"/>
-    </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="D176" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E176" s="7">
+        <v>506</v>
+      </c>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,680uF 16V 10x10 Electrolytic SMD,506</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E177" s="7">
+        <v>507</v>
+      </c>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,1000uF 10V 10x10 Electrolytic SMD,507</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E178" s="7">
+        <v>508</v>
+      </c>
+      <c r="F178" s="7"/>
+      <c r="G178" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>CAPACITORS,1500uF 6.3V 10x10 Electrolytic SMD,508</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="7"/>
+      <c r="B179" s="7"/>
+      <c r="C179" s="7"/>
       <c r="D179" s="7"/>
-    </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="7"/>
+      <c r="F179" s="7"/>
+      <c r="G179" s="7"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="7"/>
+      <c r="B180" s="7"/>
+      <c r="C180" s="7"/>
       <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
+      <c r="F180" s="7"/>
+      <c r="G180" s="7"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="7"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7"/>
+      <c r="G181" s="7"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
+      <c r="G182" s="7"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="7"/>
+      <c r="B183" s="7"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7"/>
+      <c r="G183" s="7"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="7"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7"/>
+      <c r="F184" s="7"/>
+      <c r="G184" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -13608,7 +13879,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G69" sqref="G1:G69"/>
+      <selection activeCell="E1" sqref="E1:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13639,11 +13910,11 @@
         <v>1</v>
       </c>
       <c r="E1" s="1">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G1" s="1" t="str">
         <f t="shared" ref="G1:G9" si="0">_xlfn.CONCAT(A1,",",B1," ", C1, " ",D1,",",E1)</f>
-        <v>INDUCTORS,1uH 1/2W PTH,499</v>
+        <v>INDUCTORS,1uH 1/2W PTH,509</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -13660,11 +13931,11 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="G2" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,4.7uH  1/2W PTH,500</v>
+        <v>INDUCTORS,4.7uH  1/2W PTH,510</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -13681,11 +13952,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,6.8uH 1/2W PTH,501</v>
+        <v>INDUCTORS,6.8uH 1/2W PTH,511</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -13702,11 +13973,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,10uH 1/2W PTH,502</v>
+        <v>INDUCTORS,10uH 1/2W PTH,512</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -13723,11 +13994,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,22uH 1/2W PTH,503</v>
+        <v>INDUCTORS,22uH 1/2W PTH,513</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -13744,11 +14015,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,47uH 1/2W PTH,504</v>
+        <v>INDUCTORS,47uH 1/2W PTH,514</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -13765,11 +14036,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,68uH 1/2W PTH,505</v>
+        <v>INDUCTORS,68uH 1/2W PTH,515</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -13786,11 +14057,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,100uH 1/2W PTH,506</v>
+        <v>INDUCTORS,100uH 1/2W PTH,516</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -13807,11 +14078,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>507</v>
+        <v>517</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INDUCTORS,220uH 1/2W PTH,507</v>
+        <v>INDUCTORS,220uH 1/2W PTH,517</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -13828,11 +14099,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ref="G10:G12" si="1">_xlfn.CONCAT(A10,",",B10," ", C10, " ",D10,",",E10)</f>
-        <v>INDUCTORS,330uH 1/2W PTH,508</v>
+        <v>INDUCTORS,330uH 1/2W PTH,518</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -13849,11 +14120,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>509</v>
+        <v>519</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INDUCTORS,470uH 1/2W PTH,509</v>
+        <v>INDUCTORS,470uH 1/2W PTH,519</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -13870,11 +14141,11 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INDUCTORS,1mH 1/2W PTH,510</v>
+        <v>INDUCTORS,1mH 1/2W PTH,520</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -13891,11 +14162,11 @@
         <v>226</v>
       </c>
       <c r="E13" s="1">
-        <v>511</v>
+        <v>521</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ref="G13:G21" si="2">_xlfn.CONCAT(A13,",",B13," ", C13, " ",D13,",",E13)</f>
-        <v>INDUCTORS,2.2uH (2R2) CD54 Series SMD,511</v>
+        <v>INDUCTORS,2.2uH (2R2) CD54 Series SMD,521</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -13912,11 +14183,11 @@
         <v>226</v>
       </c>
       <c r="E14" s="1">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,3.3uH (3R) CD54 Series SMD,512</v>
+        <v>INDUCTORS,3.3uH (3R) CD54 Series SMD,522</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -13933,11 +14204,11 @@
         <v>226</v>
       </c>
       <c r="E15" s="1">
-        <v>513</v>
+        <v>523</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,4.7uH (4R7) CD54 Series SMD,513</v>
+        <v>INDUCTORS,4.7uH (4R7) CD54 Series SMD,523</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -13954,11 +14225,11 @@
         <v>226</v>
       </c>
       <c r="E16" s="1">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,6.8uH (6R8) CD54 Series SMD,514</v>
+        <v>INDUCTORS,6.8uH (6R8) CD54 Series SMD,524</v>
       </c>
       <c r="H16" s="10"/>
     </row>
@@ -13976,11 +14247,11 @@
         <v>226</v>
       </c>
       <c r="E17" s="1">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,10uH (100) CD54 Series SMD,515</v>
+        <v>INDUCTORS,10uH (100) CD54 Series SMD,525</v>
       </c>
       <c r="H17" s="10"/>
     </row>
@@ -13998,11 +14269,11 @@
         <v>226</v>
       </c>
       <c r="E18" s="1">
-        <v>516</v>
+        <v>526</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,22uH (220) CD54 Series SMD,516</v>
+        <v>INDUCTORS,22uH (220) CD54 Series SMD,526</v>
       </c>
       <c r="H18" s="10"/>
     </row>
@@ -14020,11 +14291,11 @@
         <v>226</v>
       </c>
       <c r="E19" s="1">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,33uH (330) CD54 Series SMD,517</v>
+        <v>INDUCTORS,33uH (330) CD54 Series SMD,527</v>
       </c>
       <c r="H19" s="10"/>
     </row>
@@ -14042,11 +14313,11 @@
         <v>226</v>
       </c>
       <c r="E20" s="1">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,47uH (470) CD54 Series SMD,518</v>
+        <v>INDUCTORS,47uH (470) CD54 Series SMD,528</v>
       </c>
       <c r="H20" s="10"/>
     </row>
@@ -14064,11 +14335,11 @@
         <v>226</v>
       </c>
       <c r="E21" s="1">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INDUCTORS,68uH (680) CD54 Series SMD,519</v>
+        <v>INDUCTORS,68uH (680) CD54 Series SMD,529</v>
       </c>
       <c r="H21" s="10"/>
     </row>
@@ -14086,11 +14357,11 @@
         <v>226</v>
       </c>
       <c r="E22" s="1">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" ref="G22:G25" si="3">_xlfn.CONCAT(A22,",",B22," ", C22, " ",D22,",",E22)</f>
-        <v>INDUCTORS,100uH (101) CD54 Series SMD,520</v>
+        <v>INDUCTORS,100uH (101) CD54 Series SMD,530</v>
       </c>
       <c r="H22" s="10"/>
     </row>
@@ -14108,11 +14379,11 @@
         <v>226</v>
       </c>
       <c r="E23" s="1">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="G23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>INDUCTORS,220uH (221) CD54 Series SMD,521</v>
+        <v>INDUCTORS,220uH (221) CD54 Series SMD,531</v>
       </c>
       <c r="H23" s="10"/>
     </row>
@@ -14130,11 +14401,11 @@
         <v>226</v>
       </c>
       <c r="E24" s="1">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>INDUCTORS,330uH (331) CD54 Series SMD,522</v>
+        <v>INDUCTORS,330uH (331) CD54 Series SMD,532</v>
       </c>
       <c r="H24" s="10"/>
     </row>
@@ -14152,11 +14423,11 @@
         <v>226</v>
       </c>
       <c r="E25" s="1">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>INDUCTORS,470uH (471) CD54 Series SMD,523</v>
+        <v>INDUCTORS,470uH (471) CD54 Series SMD,533</v>
       </c>
       <c r="H25" s="10"/>
     </row>
@@ -14174,11 +14445,11 @@
         <v>226</v>
       </c>
       <c r="E26" s="1">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="G26" s="12" t="str">
         <f t="shared" ref="G26:G69" si="4">_xlfn.CONCAT(A26,",",B26," ", C26, " ",D26,",",E26)</f>
-        <v>INDUCTORS,4.7nH 0805 SMD,524</v>
+        <v>INDUCTORS,4.7nH 0805 SMD,534</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -14195,11 +14466,11 @@
         <v>226</v>
       </c>
       <c r="E27" s="1">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="G27" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,6.8nH 0805 SMD,525</v>
+        <v>INDUCTORS,6.8nH 0805 SMD,535</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -14216,11 +14487,11 @@
         <v>226</v>
       </c>
       <c r="E28" s="1">
-        <v>526</v>
+        <v>536</v>
       </c>
       <c r="G28" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,8.2nH 0805 SMD,526</v>
+        <v>INDUCTORS,8.2nH 0805 SMD,536</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -14237,11 +14508,11 @@
         <v>226</v>
       </c>
       <c r="E29" s="1">
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="G29" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,10nH 0805 SMD,527</v>
+        <v>INDUCTORS,10nH 0805 SMD,537</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -14258,11 +14529,11 @@
         <v>226</v>
       </c>
       <c r="E30" s="1">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="G30" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,12nH 0805 SMD,528</v>
+        <v>INDUCTORS,12nH 0805 SMD,538</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -14279,11 +14550,11 @@
         <v>226</v>
       </c>
       <c r="E31" s="1">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="G31" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,15nH 0805 SMD,529</v>
+        <v>INDUCTORS,15nH 0805 SMD,539</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -14300,11 +14571,11 @@
         <v>226</v>
       </c>
       <c r="E32" s="1">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="G32" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,18nH 0805 SMD,530</v>
+        <v>INDUCTORS,18nH 0805 SMD,540</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -14321,11 +14592,11 @@
         <v>226</v>
       </c>
       <c r="E33" s="1">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="G33" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,22nH 0805 SMD,531</v>
+        <v>INDUCTORS,22nH 0805 SMD,541</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -14342,11 +14613,11 @@
         <v>226</v>
       </c>
       <c r="E34" s="1">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="G34" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,27nH 0805 SMD,532</v>
+        <v>INDUCTORS,27nH 0805 SMD,542</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -14363,11 +14634,11 @@
         <v>226</v>
       </c>
       <c r="E35" s="1">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="G35" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,33nH 0805 SMD,533</v>
+        <v>INDUCTORS,33nH 0805 SMD,543</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -14384,11 +14655,11 @@
         <v>226</v>
       </c>
       <c r="E36" s="1">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="G36" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,39nH 0805 SMD,534</v>
+        <v>INDUCTORS,39nH 0805 SMD,544</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -14405,11 +14676,11 @@
         <v>226</v>
       </c>
       <c r="E37" s="1">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="G37" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,47nH 0805 SMD,535</v>
+        <v>INDUCTORS,47nH 0805 SMD,545</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -14426,11 +14697,11 @@
         <v>226</v>
       </c>
       <c r="E38" s="1">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="G38" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,56nH 0805 SMD,536</v>
+        <v>INDUCTORS,56nH 0805 SMD,546</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -14447,11 +14718,11 @@
         <v>226</v>
       </c>
       <c r="E39" s="1">
-        <v>537</v>
+        <v>547</v>
       </c>
       <c r="G39" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,68nH 0805 SMD,537</v>
+        <v>INDUCTORS,68nH 0805 SMD,547</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -14468,11 +14739,11 @@
         <v>226</v>
       </c>
       <c r="E40" s="1">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="G40" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,82nH 0805 SMD,538</v>
+        <v>INDUCTORS,82nH 0805 SMD,548</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -14489,11 +14760,11 @@
         <v>226</v>
       </c>
       <c r="E41" s="1">
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="G41" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,100nH 0805 SMD,539</v>
+        <v>INDUCTORS,100nH 0805 SMD,549</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -14510,11 +14781,11 @@
         <v>226</v>
       </c>
       <c r="E42" s="1">
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="G42" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,120nH 0805 SMD,540</v>
+        <v>INDUCTORS,120nH 0805 SMD,550</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -14531,11 +14802,11 @@
         <v>226</v>
       </c>
       <c r="E43" s="1">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="G43" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,150nH 0805 SMD,541</v>
+        <v>INDUCTORS,150nH 0805 SMD,551</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -14552,11 +14823,11 @@
         <v>226</v>
       </c>
       <c r="E44" s="1">
-        <v>542</v>
+        <v>552</v>
       </c>
       <c r="G44" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,220nH 0805 SMD,542</v>
+        <v>INDUCTORS,220nH 0805 SMD,552</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -14573,11 +14844,11 @@
         <v>226</v>
       </c>
       <c r="E45" s="1">
-        <v>543</v>
+        <v>553</v>
       </c>
       <c r="G45" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,270nH 0805 SMD,543</v>
+        <v>INDUCTORS,270nH 0805 SMD,553</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -14594,11 +14865,11 @@
         <v>226</v>
       </c>
       <c r="E46" s="1">
-        <v>544</v>
+        <v>554</v>
       </c>
       <c r="G46" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,330nH 0805 SMD,544</v>
+        <v>INDUCTORS,330nH 0805 SMD,554</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -14615,11 +14886,11 @@
         <v>226</v>
       </c>
       <c r="E47" s="1">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="G47" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,470nH 0805 SMD,545</v>
+        <v>INDUCTORS,470nH 0805 SMD,555</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -14636,11 +14907,11 @@
         <v>226</v>
       </c>
       <c r="E48" s="1">
-        <v>546</v>
+        <v>556</v>
       </c>
       <c r="G48" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,560nH 0805 SMD,546</v>
+        <v>INDUCTORS,560nH 0805 SMD,556</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -14657,11 +14928,11 @@
         <v>226</v>
       </c>
       <c r="E49" s="1">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="G49" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,680nH 0805 SMD,547</v>
+        <v>INDUCTORS,680nH 0805 SMD,557</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -14678,11 +14949,11 @@
         <v>226</v>
       </c>
       <c r="E50" s="1">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="G50" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,820nH 0805 SMD,548</v>
+        <v>INDUCTORS,820nH 0805 SMD,558</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -14699,11 +14970,11 @@
         <v>226</v>
       </c>
       <c r="E51" s="1">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="G51" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,1.0uH 0805 SMD,549</v>
+        <v>INDUCTORS,1.0uH 0805 SMD,559</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -14720,11 +14991,11 @@
         <v>226</v>
       </c>
       <c r="E52" s="1">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="G52" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,1.2uH 0805 SMD,550</v>
+        <v>INDUCTORS,1.2uH 0805 SMD,560</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -14741,11 +15012,11 @@
         <v>226</v>
       </c>
       <c r="E53" s="1">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G53" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,1.5uH 0805 SMD,551</v>
+        <v>INDUCTORS,1.5uH 0805 SMD,561</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -14762,11 +15033,11 @@
         <v>226</v>
       </c>
       <c r="E54" s="1">
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="G54" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,1.8uH 0805 SMD,552</v>
+        <v>INDUCTORS,1.8uH 0805 SMD,562</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -14783,11 +15054,11 @@
         <v>226</v>
       </c>
       <c r="E55" s="1">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="G55" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,2.2uH 0805 SMD,553</v>
+        <v>INDUCTORS,2.2uH 0805 SMD,563</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -14804,11 +15075,11 @@
         <v>226</v>
       </c>
       <c r="E56" s="1">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="G56" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,2.7uH 0805 SMD,554</v>
+        <v>INDUCTORS,2.7uH 0805 SMD,564</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -14825,11 +15096,11 @@
         <v>226</v>
       </c>
       <c r="E57" s="1">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="G57" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,3.3uH 0805 SMD,555</v>
+        <v>INDUCTORS,3.3uH 0805 SMD,565</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -14846,11 +15117,11 @@
         <v>226</v>
       </c>
       <c r="E58" s="1">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="G58" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,4.7uH 0805 SMD,556</v>
+        <v>INDUCTORS,4.7uH 0805 SMD,566</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -14867,11 +15138,11 @@
         <v>226</v>
       </c>
       <c r="E59" s="1">
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="G59" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,5.6uH 0805 SMD,557</v>
+        <v>INDUCTORS,5.6uH 0805 SMD,567</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -14888,11 +15159,11 @@
         <v>226</v>
       </c>
       <c r="E60" s="1">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="G60" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,6.8uH 0805 SMD,558</v>
+        <v>INDUCTORS,6.8uH 0805 SMD,568</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -14909,11 +15180,11 @@
         <v>226</v>
       </c>
       <c r="E61" s="1">
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="G61" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,8.2uH 0805 SMD,559</v>
+        <v>INDUCTORS,8.2uH 0805 SMD,569</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -14930,11 +15201,11 @@
         <v>226</v>
       </c>
       <c r="E62" s="1">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="G62" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,10uH 0805 SMD,560</v>
+        <v>INDUCTORS,10uH 0805 SMD,570</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -14951,11 +15222,11 @@
         <v>226</v>
       </c>
       <c r="E63" s="1">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="G63" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,12uH 0805 SMD,561</v>
+        <v>INDUCTORS,12uH 0805 SMD,571</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -14972,11 +15243,11 @@
         <v>226</v>
       </c>
       <c r="E64" s="1">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="G64" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,15uH 0805 SMD,562</v>
+        <v>INDUCTORS,15uH 0805 SMD,572</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -14993,11 +15264,11 @@
         <v>226</v>
       </c>
       <c r="E65" s="1">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="G65" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,18uH 0805 SMD,563</v>
+        <v>INDUCTORS,18uH 0805 SMD,573</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -15014,11 +15285,11 @@
         <v>226</v>
       </c>
       <c r="E66" s="1">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="G66" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,22uH 0805 SMD,564</v>
+        <v>INDUCTORS,22uH 0805 SMD,574</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -15035,11 +15306,11 @@
         <v>226</v>
       </c>
       <c r="E67" s="1">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="G67" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,33uH 0805 SMD,565</v>
+        <v>INDUCTORS,33uH 0805 SMD,575</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -15056,11 +15327,11 @@
         <v>226</v>
       </c>
       <c r="E68" s="1">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="G68" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,47uH 0805 SMD,566</v>
+        <v>INDUCTORS,47uH 0805 SMD,576</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -15077,11 +15348,11 @@
         <v>226</v>
       </c>
       <c r="E69" s="1">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="G69" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>INDUCTORS,100uH 0805 SMD,567</v>
+        <v>INDUCTORS,100uH 0805 SMD,577</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>